<commit_message>
Able to store/load songs via excel
</commit_message>
<xml_diff>
--- a/public/data/songs.xlsx
+++ b/public/data/songs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Devry\CEIS209\Mckinney_CourseProject_CEIS209\public\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1E355E08-97F9-4D19-95BC-87D5B5B4FF0D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8F86D54-C93F-4170-B940-D7A76889D59B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-19310" yWindow="4780" windowWidth="19420" windowHeight="10420" xr2:uid="{F7B10C41-70EF-4519-8A6C-AFDFA81AC790}"/>
+    <workbookView xWindow="-19310" yWindow="4780" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -53,91 +53,91 @@
     <t>URL</t>
   </si>
   <si>
+    <t>Dubstep</t>
+  </si>
+  <si>
+    <t>Matafaka</t>
+  </si>
+  <si>
+    <t>Unknown Brain Feat. Marvin Divine</t>
+  </si>
+  <si>
+    <t>Pulsar</t>
+  </si>
+  <si>
+    <t>Animadrop</t>
+  </si>
+  <si>
+    <t>Evanescence</t>
+  </si>
+  <si>
+    <t>https://youtu.be/AlXfbVpDUdo</t>
+  </si>
+  <si>
+    <t>https://youtu.be/2UC7Q0_5Vuc</t>
+  </si>
+  <si>
+    <t>https://youtu.be/Viwd2P5fJZA</t>
+  </si>
+  <si>
+    <t>MyKool</t>
+  </si>
+  <si>
+    <t>Ikiru</t>
+  </si>
+  <si>
+    <t>ChillStep</t>
+  </si>
+  <si>
+    <t>https://youtu.be/bfRNYRcQugs</t>
+  </si>
+  <si>
+    <t>Possibilities</t>
+  </si>
+  <si>
+    <t>Melodysheep</t>
+  </si>
+  <si>
+    <t>Electro</t>
+  </si>
+  <si>
+    <t>https://youtu.be/x49mJDdcGYg</t>
+  </si>
+  <si>
+    <t>https://youtu.be/HnE9mQ4XibE</t>
+  </si>
+  <si>
+    <t>Tristam &amp; Braken</t>
+  </si>
+  <si>
+    <t>Techno</t>
+  </si>
+  <si>
+    <t>https://youtu.be/M-P4QBt-FWw</t>
+  </si>
+  <si>
+    <t>House</t>
+  </si>
+  <si>
+    <t>Dark Side</t>
+  </si>
+  <si>
+    <t>Alan Walker (feat. Au/Ra and Tomine Harket)</t>
+  </si>
+  <si>
     <t>Mortals</t>
   </si>
   <si>
     <t>Warriyo Feat. Laura Brehm</t>
   </si>
   <si>
-    <t>Dubstep</t>
-  </si>
-  <si>
-    <t>Matafaka</t>
-  </si>
-  <si>
-    <t>Unknown Brain Feat. Marvin Divine</t>
-  </si>
-  <si>
-    <t>Pulsar</t>
-  </si>
-  <si>
-    <t>Animadrop</t>
-  </si>
-  <si>
-    <t>Bring Me To Life (Terminite &amp; The Arcturians Remix)</t>
-  </si>
-  <si>
-    <t>Evanescence</t>
-  </si>
-  <si>
     <t>https://youtu.be/yJg-Y5byMMw</t>
   </si>
   <si>
-    <t>https://youtu.be/AlXfbVpDUdo</t>
-  </si>
-  <si>
-    <t>https://youtu.be/2UC7Q0_5Vuc</t>
-  </si>
-  <si>
-    <t>https://youtu.be/Viwd2P5fJZA</t>
-  </si>
-  <si>
-    <t>MyKool</t>
-  </si>
-  <si>
-    <t>Ikiru</t>
-  </si>
-  <si>
-    <t>ChillStep</t>
-  </si>
-  <si>
-    <t>https://youtu.be/bfRNYRcQugs</t>
-  </si>
-  <si>
-    <t>Possibilities</t>
-  </si>
-  <si>
-    <t>Melodysheep</t>
-  </si>
-  <si>
-    <t>Electro</t>
-  </si>
-  <si>
-    <t>https://youtu.be/x49mJDdcGYg</t>
-  </si>
-  <si>
-    <t>https://youtu.be/HnE9mQ4XibE</t>
-  </si>
-  <si>
-    <t>Tristam &amp; Braken</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Flight (EXO TERROR Remix) </t>
-  </si>
-  <si>
-    <t>Techno</t>
-  </si>
-  <si>
-    <t>https://youtu.be/M-P4QBt-FWw</t>
-  </si>
-  <si>
-    <t>House</t>
-  </si>
-  <si>
-    <t>Dark Side</t>
-  </si>
-  <si>
-    <t>Alan Walker (feat. Au/Ra and Tomine Harket)</t>
+    <t xml:space="preserve"> Flight</t>
+  </si>
+  <si>
+    <t>Bring Me To Life</t>
   </si>
 </sst>
 </file>
@@ -180,7 +180,7 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -499,11 +499,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B0033071-62E2-4AF3-A920-9417FDA3E064}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -532,147 +532,148 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C2" t="s">
         <v>5</v>
-      </c>
-      <c r="B2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2" t="s">
-        <v>7</v>
       </c>
       <c r="D2">
         <v>2020</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>14</v>
+        <v>31</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B3" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C3" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D3">
         <v>2020</v>
       </c>
       <c r="E3" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B4" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C4" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D4">
         <v>2020</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>12</v>
+        <v>33</v>
       </c>
       <c r="B5" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="C5" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D5">
         <v>2020</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="B6" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="C6" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="D6">
         <v>2015</v>
       </c>
       <c r="E6" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="B7" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="C7" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="D7">
         <v>2021</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="B8" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="C8" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="D8">
         <v>2018</v>
       </c>
       <c r="E8" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="B9" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="C9" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="D9">
         <v>2018</v>
       </c>
       <c r="E9" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E7" r:id="rId1" xr:uid="{FC1DE50E-4F97-4B95-9086-0D30D716418D}"/>
-    <hyperlink ref="E5" r:id="rId2" xr:uid="{5BE97892-BE12-42E1-BF48-11240411D349}"/>
-    <hyperlink ref="E4" r:id="rId3" xr:uid="{2EA23166-1B60-4E33-8C42-AAAF7E9DC6E5}"/>
+    <hyperlink ref="E7" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="E5" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="E4" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="E2" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId4"/>
+  <pageSetup orientation="portrait" r:id="rId5"/>
 </worksheet>
 </file>
</xml_diff>